<commit_message>
Updated experimental data and integrated some reports.
</commit_message>
<xml_diff>
--- a/3.a.SentenceBert/splitSentenceBertCluster/finalGroup_0.xlsx
+++ b/3.a.SentenceBert/splitSentenceBertCluster/finalGroup_0.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Word Frequency" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="finalGroup_0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="finalGroup_0_WF" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>